<commit_message>
changed paths according to new library name, python-Modelica interface tested
</commit_message>
<xml_diff>
--- a/PyScripts/output/validation.xlsx
+++ b/PyScripts/output/validation.xlsx
@@ -1,13 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <workbookProtection/>
   <bookViews>
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>

</xml_diff>

<commit_message>
major update: extended all mass trasnfer components to work with generic fluid model (not only MoistAir) - successfully tested for aircraft application
</commit_message>
<xml_diff>
--- a/PyScripts/output/validation.xlsx
+++ b/PyScripts/output/validation.xlsx
@@ -451,13 +451,13 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>51123.40844377594</v>
+        <v>51123.40844082075</v>
       </c>
       <c r="C2" t="n">
-        <v>33002.49716568398</v>
+        <v>33002.49715192382</v>
       </c>
       <c r="D2" t="n">
-        <v>30867.07844387362</v>
+        <v>30867.07844387506</v>
       </c>
     </row>
     <row r="3">
@@ -467,13 +467,13 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>32151.95454614695</v>
+        <v>32151.95454438015</v>
       </c>
       <c r="C3" t="n">
-        <v>22868.41210372771</v>
+        <v>22868.41210371276</v>
       </c>
       <c r="D3" t="n">
-        <v>24207.26828665564</v>
+        <v>24207.26828665595</v>
       </c>
     </row>
     <row r="4">
@@ -489,7 +489,7 @@
         <v>28159.8542017977</v>
       </c>
       <c r="D4" t="n">
-        <v>28159.85420179771</v>
+        <v>28159.8542017977</v>
       </c>
     </row>
     <row r="5">
@@ -499,13 +499,13 @@
         </is>
       </c>
       <c r="B5" t="n">
-        <v>1832.100344349248</v>
+        <v>1832.100342582449</v>
       </c>
       <c r="C5" t="n">
-        <v>-5291.442098069987</v>
+        <v>-5291.442098084946</v>
       </c>
       <c r="D5" t="n">
-        <v>-3952.585915142063</v>
+        <v>-3952.585915141754</v>
       </c>
     </row>
     <row r="6">
@@ -515,13 +515,13 @@
         </is>
       </c>
       <c r="B6" t="n">
-        <v>3479.54460249962</v>
+        <v>3479.544605190089</v>
       </c>
       <c r="C6" t="n">
-        <v>593.750732687784</v>
+        <v>593.7507326833602</v>
       </c>
       <c r="D6" t="n">
-        <v>844.1348722810862</v>
+        <v>844.1348722981538</v>
       </c>
     </row>
     <row r="7">
@@ -547,13 +547,13 @@
         </is>
       </c>
       <c r="B8" t="n">
-        <v>1912.04460249962</v>
+        <v>1912.044605190089</v>
       </c>
       <c r="C8" t="n">
-        <v>-973.749267312216</v>
+        <v>-973.7492673166398</v>
       </c>
       <c r="D8" t="n">
-        <v>-723.3651277189138</v>
+        <v>-723.3651277018462</v>
       </c>
     </row>
     <row r="9">
@@ -579,13 +579,13 @@
         </is>
       </c>
       <c r="B10" t="n">
-        <v>26.99999999985204</v>
+        <v>27.00000000000648</v>
       </c>
       <c r="C10" t="n">
-        <v>23.92201599253337</v>
+        <v>23.9220159925294</v>
       </c>
       <c r="D10" t="n">
-        <v>27.0506872445028</v>
+        <v>27.05068724456487</v>
       </c>
     </row>
     <row r="11">
@@ -595,13 +595,13 @@
         </is>
       </c>
       <c r="B11" t="n">
-        <v>27.06493257686435</v>
+        <v>27.06493257702311</v>
       </c>
       <c r="C11" t="n">
         <v>23.99999999999989</v>
       </c>
       <c r="D11" t="n">
-        <v>26.99999999999966</v>
+        <v>27.00000000000011</v>
       </c>
     </row>
     <row r="12">
@@ -611,10 +611,10 @@
         </is>
       </c>
       <c r="B12" t="n">
-        <v>27.44823575512982</v>
+        <v>27.44823575467154</v>
       </c>
       <c r="C12" t="n">
-        <v>23.25858522805038</v>
+        <v>23.25858522805044</v>
       </c>
       <c r="D12" t="n">
         <v>26.34616545357073</v>
@@ -627,13 +627,13 @@
         </is>
       </c>
       <c r="B13" t="n">
-        <v>64.05080512837509</v>
+        <v>64.05080512713528</v>
       </c>
       <c r="C13" t="n">
-        <v>22.46863165580305</v>
+        <v>22.46863165580055</v>
       </c>
       <c r="D13" t="n">
-        <v>25.80292781417836</v>
+        <v>25.8029278142273</v>
       </c>
     </row>
     <row r="14">
@@ -643,13 +643,13 @@
         </is>
       </c>
       <c r="B14" t="n">
-        <v>12.18548261695429</v>
+        <v>12.18548261925031</v>
       </c>
       <c r="C14" t="n">
-        <v>16.08586184513837</v>
+        <v>16.08586184513888</v>
       </c>
       <c r="D14" t="n">
-        <v>16.56164412922283</v>
+        <v>16.56164412922658</v>
       </c>
     </row>
     <row r="15">
@@ -659,13 +659,13 @@
         </is>
       </c>
       <c r="B15" t="n">
-        <v>8.394332547675134</v>
+        <v>8.394332575371465</v>
       </c>
       <c r="C15" t="n">
-        <v>6.515936818817853</v>
+        <v>6.515936818824304</v>
       </c>
       <c r="D15" t="n">
-        <v>6.317076441765987</v>
+        <v>6.317076441746626</v>
       </c>
     </row>
     <row r="16">
@@ -675,13 +675,13 @@
         </is>
       </c>
       <c r="B16" t="n">
-        <v>15.07337725223902</v>
+        <v>15.07337725599263</v>
       </c>
       <c r="C16" t="n">
-        <v>12.44247362313206</v>
+        <v>12.44247362313205</v>
       </c>
       <c r="D16" t="n">
-        <v>12.32740067044918</v>
+        <v>12.32740067044879</v>
       </c>
     </row>
     <row r="17">
@@ -691,13 +691,13 @@
         </is>
       </c>
       <c r="B17" t="n">
-        <v>14.71240470807509</v>
+        <v>14.71240471012513</v>
       </c>
       <c r="C17" t="n">
-        <v>12.97836966133781</v>
+        <v>12.97836966133772</v>
       </c>
       <c r="D17" t="n">
-        <v>12.78456808977975</v>
+        <v>12.78456808977965</v>
       </c>
     </row>
     <row r="18">
@@ -707,13 +707,13 @@
         </is>
       </c>
       <c r="B18" t="n">
-        <v>1.247770099937178</v>
+        <v>1.247770103674462</v>
       </c>
       <c r="C18" t="n">
-        <v>7.112039717400428</v>
+        <v>7.112039717408187</v>
       </c>
       <c r="D18" t="n">
-        <v>6.797671810005921</v>
+        <v>6.797671809991044</v>
       </c>
     </row>
     <row r="19">
@@ -723,13 +723,13 @@
         </is>
       </c>
       <c r="B19" t="n">
-        <v>2.000000000001329</v>
+        <v>2.000000000000652</v>
       </c>
       <c r="C19" t="n">
-        <v>2.119999999999993</v>
+        <v>2.119999999999991</v>
       </c>
       <c r="D19" t="n">
-        <v>1.759999999999859</v>
+        <v>1.759999999999832</v>
       </c>
     </row>
     <row r="20">
@@ -739,13 +739,13 @@
         </is>
       </c>
       <c r="B20" t="n">
-        <v>0.2234880159033935</v>
+        <v>0.2234880159044185</v>
       </c>
       <c r="C20" t="n">
-        <v>0.2383397257422269</v>
+        <v>0.2383397257422257</v>
       </c>
       <c r="D20" t="n">
-        <v>0.2010463604263795</v>
+        <v>0.2010463604263769</v>
       </c>
     </row>
     <row r="21">
@@ -755,13 +755,13 @@
         </is>
       </c>
       <c r="B21" t="n">
-        <v>1.811511984097935</v>
+        <v>1.811511984096234</v>
       </c>
       <c r="C21" t="n">
-        <v>1.898660274257767</v>
+        <v>1.898660274257765</v>
       </c>
       <c r="D21" t="n">
-        <v>1.575953639573479</v>
+        <v>1.575953639573455</v>
       </c>
     </row>
     <row r="22">
@@ -771,13 +771,13 @@
         </is>
       </c>
       <c r="B22" t="n">
-        <v>1.814700724487775</v>
+        <v>1.814700724491995</v>
       </c>
       <c r="C22" t="n">
-        <v>1.901707016011351</v>
+        <v>1.901707016010914</v>
       </c>
       <c r="D22" t="n">
-        <v>1.578955118264566</v>
+        <v>1.578955118264712</v>
       </c>
     </row>
     <row r="23">
@@ -835,13 +835,13 @@
         </is>
       </c>
       <c r="B26" t="n">
-        <v>0.1258015807964699</v>
+        <v>0.1258015807971674</v>
       </c>
       <c r="C26" t="n">
-        <v>0.116576792985651</v>
+        <v>0.1165767929856504</v>
       </c>
       <c r="D26" t="n">
-        <v>0.1167841209314954</v>
+        <v>0.1167841209314955</v>
       </c>
     </row>
     <row r="27">
@@ -915,13 +915,13 @@
         </is>
       </c>
       <c r="B31" t="n">
-        <v>104.9335067650732</v>
+        <v>104.9335067650825</v>
       </c>
       <c r="C31" t="n">
-        <v>79.90350915201587</v>
+        <v>79.90350915201584</v>
       </c>
       <c r="D31" t="n">
-        <v>78.81054667555547</v>
+        <v>78.81054667555541</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
updated pipe model, added distinction between circular and rectangular section, added distributed heat ports, steady-state aircraft model working, dynamic has problem with initialization
</commit_message>
<xml_diff>
--- a/PyScripts/output/validation.xlsx
+++ b/PyScripts/output/validation.xlsx
@@ -451,13 +451,13 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>51123.40844082075</v>
+        <v>50709.26919481565</v>
       </c>
       <c r="C2" t="n">
-        <v>33002.49715192382</v>
+        <v>32436.48727425859</v>
       </c>
       <c r="D2" t="n">
-        <v>30867.07844387506</v>
+        <v>30527.88561606283</v>
       </c>
     </row>
     <row r="3">
@@ -467,13 +467,13 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>32151.95454438015</v>
+        <v>32192.30262320694</v>
       </c>
       <c r="C3" t="n">
-        <v>22868.41210371276</v>
+        <v>22866.78012130396</v>
       </c>
       <c r="D3" t="n">
-        <v>24207.26828665595</v>
+        <v>24205.3779859723</v>
       </c>
     </row>
     <row r="4">
@@ -499,13 +499,13 @@
         </is>
       </c>
       <c r="B5" t="n">
-        <v>1832.100342582449</v>
+        <v>1872.448421409234</v>
       </c>
       <c r="C5" t="n">
-        <v>-5291.442098084946</v>
+        <v>-5293.074080493738</v>
       </c>
       <c r="D5" t="n">
-        <v>-3952.585915141754</v>
+        <v>-3954.476215825402</v>
       </c>
     </row>
     <row r="6">
@@ -515,13 +515,13 @@
         </is>
       </c>
       <c r="B6" t="n">
-        <v>3479.544605190089</v>
+        <v>3504.077841354558</v>
       </c>
       <c r="C6" t="n">
-        <v>593.7507326833602</v>
+        <v>600.0792247045911</v>
       </c>
       <c r="D6" t="n">
-        <v>844.1348722981538</v>
+        <v>851.4687391656371</v>
       </c>
     </row>
     <row r="7">
@@ -547,13 +547,13 @@
         </is>
       </c>
       <c r="B8" t="n">
-        <v>1912.044605190089</v>
+        <v>1936.577841354558</v>
       </c>
       <c r="C8" t="n">
-        <v>-973.7492673166398</v>
+        <v>-967.4207752954089</v>
       </c>
       <c r="D8" t="n">
-        <v>-723.3651277018462</v>
+        <v>-716.0312608343629</v>
       </c>
     </row>
     <row r="9">
@@ -563,13 +563,13 @@
         </is>
       </c>
       <c r="B9" t="n">
-        <v>-13.58222045898435</v>
+        <v>-13.57724609374998</v>
       </c>
       <c r="C9" t="n">
-        <v>-1.646612548828102</v>
+        <v>-1.139196777343727</v>
       </c>
       <c r="D9" t="n">
-        <v>-1.241308593749977</v>
+        <v>-0.8878845214843523</v>
       </c>
     </row>
     <row r="10">
@@ -579,13 +579,13 @@
         </is>
       </c>
       <c r="B10" t="n">
-        <v>27.00000000000648</v>
+        <v>26.99999999997857</v>
       </c>
       <c r="C10" t="n">
-        <v>23.9220159925294</v>
+        <v>23.71977692081987</v>
       </c>
       <c r="D10" t="n">
-        <v>27.05068724456487</v>
+        <v>26.79777666228358</v>
       </c>
     </row>
     <row r="11">
@@ -595,13 +595,13 @@
         </is>
       </c>
       <c r="B11" t="n">
-        <v>27.06493257702311</v>
+        <v>26.63446859944048</v>
       </c>
       <c r="C11" t="n">
-        <v>23.99999999999989</v>
+        <v>23.99999999999972</v>
       </c>
       <c r="D11" t="n">
-        <v>27.00000000000011</v>
+        <v>26.99999999995276</v>
       </c>
     </row>
     <row r="12">
@@ -611,13 +611,13 @@
         </is>
       </c>
       <c r="B12" t="n">
-        <v>27.44823575467154</v>
+        <v>27.02262291110753</v>
       </c>
       <c r="C12" t="n">
-        <v>23.25858522805044</v>
+        <v>23.25632273469279</v>
       </c>
       <c r="D12" t="n">
-        <v>26.34616545357073</v>
+        <v>26.34428433441923</v>
       </c>
     </row>
     <row r="13">
@@ -627,13 +627,13 @@
         </is>
       </c>
       <c r="B13" t="n">
-        <v>64.05080512713528</v>
+        <v>64.68334894098598</v>
       </c>
       <c r="C13" t="n">
-        <v>22.46863165580055</v>
+        <v>22.30279351510057</v>
       </c>
       <c r="D13" t="n">
-        <v>25.8029278142273</v>
+        <v>25.58199758956857</v>
       </c>
     </row>
     <row r="14">
@@ -643,13 +643,13 @@
         </is>
       </c>
       <c r="B14" t="n">
-        <v>12.18548261925031</v>
+        <v>11.76268661558453</v>
       </c>
       <c r="C14" t="n">
-        <v>16.08586184513888</v>
+        <v>16.05967017558862</v>
       </c>
       <c r="D14" t="n">
-        <v>16.56164412922658</v>
+        <v>16.52853569592492</v>
       </c>
     </row>
     <row r="15">
@@ -659,13 +659,13 @@
         </is>
       </c>
       <c r="B15" t="n">
-        <v>8.394332575371465</v>
+        <v>8.42226987810564</v>
       </c>
       <c r="C15" t="n">
-        <v>6.515936818824304</v>
+        <v>6.579533647300682</v>
       </c>
       <c r="D15" t="n">
-        <v>6.317076441746626</v>
+        <v>6.398559916072532</v>
       </c>
     </row>
     <row r="16">
@@ -675,13 +675,13 @@
         </is>
       </c>
       <c r="B16" t="n">
-        <v>15.07337725599263</v>
+        <v>15.44572833419447</v>
       </c>
       <c r="C16" t="n">
-        <v>12.44247362313205</v>
+        <v>12.46304688888272</v>
       </c>
       <c r="D16" t="n">
-        <v>12.32740067044879</v>
+        <v>12.3467559851574</v>
       </c>
     </row>
     <row r="17">
@@ -691,13 +691,13 @@
         </is>
       </c>
       <c r="B17" t="n">
-        <v>14.71240471012513</v>
+        <v>15.07037301409483</v>
       </c>
       <c r="C17" t="n">
-        <v>12.97836966133772</v>
+        <v>13.00171485776169</v>
       </c>
       <c r="D17" t="n">
-        <v>12.78456808977965</v>
+        <v>12.80614804761802</v>
       </c>
     </row>
     <row r="18">
@@ -707,13 +707,13 @@
         </is>
       </c>
       <c r="B18" t="n">
-        <v>1.247770103674462</v>
+        <v>1.216857408920424</v>
       </c>
       <c r="C18" t="n">
-        <v>7.112039717408187</v>
+        <v>7.166476143855323</v>
       </c>
       <c r="D18" t="n">
-        <v>6.797671809991044</v>
+        <v>6.873220772578689</v>
       </c>
     </row>
     <row r="19">
@@ -723,13 +723,13 @@
         </is>
       </c>
       <c r="B19" t="n">
-        <v>2.000000000000652</v>
+        <v>1.999999999999922</v>
       </c>
       <c r="C19" t="n">
-        <v>2.119999999999991</v>
+        <v>2.120000000000009</v>
       </c>
       <c r="D19" t="n">
-        <v>1.759999999999832</v>
+        <v>1.760000000014667</v>
       </c>
     </row>
     <row r="20">
@@ -739,13 +739,13 @@
         </is>
       </c>
       <c r="B20" t="n">
-        <v>0.2234880159044185</v>
+        <v>0.218890967250746</v>
       </c>
       <c r="C20" t="n">
-        <v>0.2383397257422257</v>
+        <v>0.2446960102280806</v>
       </c>
       <c r="D20" t="n">
-        <v>0.2010463604263769</v>
+        <v>0.2061137846734573</v>
       </c>
     </row>
     <row r="21">
@@ -755,13 +755,13 @@
         </is>
       </c>
       <c r="B21" t="n">
-        <v>1.811511984096234</v>
+        <v>1.816109032749176</v>
       </c>
       <c r="C21" t="n">
-        <v>1.898660274257765</v>
+        <v>1.892303989771928</v>
       </c>
       <c r="D21" t="n">
-        <v>1.575953639573455</v>
+        <v>1.57088621534121</v>
       </c>
     </row>
     <row r="22">
@@ -771,13 +771,13 @@
         </is>
       </c>
       <c r="B22" t="n">
-        <v>1.814700724491995</v>
+        <v>1.819299135049805</v>
       </c>
       <c r="C22" t="n">
-        <v>1.901707016010914</v>
+        <v>1.895350387741783</v>
       </c>
       <c r="D22" t="n">
-        <v>1.578955118264712</v>
+        <v>1.573887308414705</v>
       </c>
     </row>
     <row r="23">
@@ -787,13 +787,13 @@
         </is>
       </c>
       <c r="B23" t="n">
-        <v>0.2235465794801712</v>
+        <v>0.2189495116472244</v>
       </c>
       <c r="C23" t="n">
-        <v>0.2383994162082672</v>
+        <v>0.2447557151317596</v>
       </c>
       <c r="D23" t="n">
-        <v>0.201105609536171</v>
+        <v>0.2061730474233627</v>
       </c>
     </row>
     <row r="24">
@@ -819,13 +819,13 @@
         </is>
       </c>
       <c r="B25" t="n">
-        <v>1.038247346878052</v>
+        <v>1.038248658180237</v>
       </c>
       <c r="C25" t="n">
-        <v>1.080106377601624</v>
+        <v>1.080106139183044</v>
       </c>
       <c r="D25" t="n">
-        <v>0.9000607132911682</v>
+        <v>0.9000603556632996</v>
       </c>
     </row>
     <row r="26">
@@ -835,13 +835,13 @@
         </is>
       </c>
       <c r="B26" t="n">
-        <v>0.1258015807971674</v>
+        <v>0.1228958829729158</v>
       </c>
       <c r="C26" t="n">
-        <v>0.1165767929856504</v>
+        <v>0.1203273953121686</v>
       </c>
       <c r="D26" t="n">
-        <v>0.1167841209314955</v>
+        <v>0.1203866854432739</v>
       </c>
     </row>
     <row r="27">
@@ -883,13 +883,13 @@
         </is>
       </c>
       <c r="B29" t="n">
-        <v>104.9335078125</v>
+        <v>104.5986171875</v>
       </c>
       <c r="C29" t="n">
-        <v>79.9035078125</v>
+        <v>79.60111718749999</v>
       </c>
       <c r="D29" t="n">
-        <v>78.810546875</v>
+        <v>78.59155468749999</v>
       </c>
     </row>
     <row r="30">
@@ -899,13 +899,13 @@
         </is>
       </c>
       <c r="B30" t="n">
-        <v>100.14353125</v>
+        <v>100.1430703125</v>
       </c>
       <c r="C30" t="n">
-        <v>73.88982812499999</v>
+        <v>73.89046875</v>
       </c>
       <c r="D30" t="n">
-        <v>74.2821015625</v>
+        <v>74.28260937500001</v>
       </c>
     </row>
     <row r="31">
@@ -915,13 +915,13 @@
         </is>
       </c>
       <c r="B31" t="n">
-        <v>104.9335067650825</v>
+        <v>104.5986147265888</v>
       </c>
       <c r="C31" t="n">
-        <v>79.90350915201584</v>
+        <v>79.60111683149745</v>
       </c>
       <c r="D31" t="n">
-        <v>78.81054667555541</v>
+        <v>78.59155668363148</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Improved environment model, implemented thermal_distributed and heatFlowMultiplier, fixed all Tests except for Distributed
</commit_message>
<xml_diff>
--- a/PyScripts/output/validation.xlsx
+++ b/PyScripts/output/validation.xlsx
@@ -451,7 +451,7 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>51299.77620886141</v>
+        <v>51005.00823254297</v>
       </c>
       <c r="C2" t="n">
         <v>32470.46482413697</v>
@@ -467,7 +467,7 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>32633.97734808491</v>
+        <v>32401.14538257632</v>
       </c>
       <c r="C3" t="n">
         <v>22890.15223737805</v>
@@ -499,7 +499,7 @@
         </is>
       </c>
       <c r="B5" t="n">
-        <v>2314.123146287206</v>
+        <v>2081.291180778615</v>
       </c>
       <c r="C5" t="n">
         <v>-5269.701964419652</v>
@@ -515,7 +515,7 @@
         </is>
       </c>
       <c r="B6" t="n">
-        <v>3596.202853792583</v>
+        <v>3532.226790597309</v>
       </c>
       <c r="C6" t="n">
         <v>603.2279645160052</v>
@@ -547,7 +547,7 @@
         </is>
       </c>
       <c r="B8" t="n">
-        <v>2028.702853792583</v>
+        <v>1964.726790597309</v>
       </c>
       <c r="C8" t="n">
         <v>-964.2720354839948</v>
@@ -563,7 +563,7 @@
         </is>
       </c>
       <c r="B9" t="n">
-        <v>-14.2883361816406</v>
+        <v>-13.85159912109373</v>
       </c>
       <c r="C9" t="n">
         <v>-1.167364501953102</v>
@@ -579,7 +579,7 @@
         </is>
       </c>
       <c r="B10" t="n">
-        <v>26.99999999999983</v>
+        <v>26.99999999998431</v>
       </c>
       <c r="C10" t="n">
         <v>23.72113514408119</v>
@@ -595,7 +595,7 @@
         </is>
       </c>
       <c r="B11" t="n">
-        <v>26.46706608240203</v>
+        <v>26.62374482422558</v>
       </c>
       <c r="C11" t="n">
         <v>23.99999999999983</v>
@@ -611,7 +611,7 @@
         </is>
       </c>
       <c r="B12" t="n">
-        <v>26.88362262949369</v>
+        <v>27.03821225603286</v>
       </c>
       <c r="C12" t="n">
         <v>23.25952019118625</v>
@@ -627,7 +627,7 @@
         </is>
       </c>
       <c r="B13" t="n">
-        <v>64.73349270889196</v>
+        <v>64.73487797803335</v>
       </c>
       <c r="C13" t="n">
         <v>22.31024172486366</v>
@@ -643,7 +643,7 @@
         </is>
       </c>
       <c r="B14" t="n">
-        <v>11.34512000809707</v>
+        <v>11.63509226463992</v>
       </c>
       <c r="C14" t="n">
         <v>16.04738618027744</v>
@@ -659,7 +659,7 @@
         </is>
       </c>
       <c r="B15" t="n">
-        <v>8.423013137011665</v>
+        <v>8.422298003455047</v>
       </c>
       <c r="C15" t="n">
         <v>6.578993866641933</v>
@@ -675,7 +675,7 @@
         </is>
       </c>
       <c r="B16" t="n">
-        <v>15.6007048102111</v>
+        <v>15.45561770905346</v>
       </c>
       <c r="C16" t="n">
         <v>12.46304758374061</v>
@@ -691,7 +691,7 @@
         </is>
       </c>
       <c r="B17" t="n">
-        <v>15.19575318482976</v>
+        <v>15.05671624322933</v>
       </c>
       <c r="C17" t="n">
         <v>12.99920415303144</v>
@@ -707,7 +707,7 @@
         </is>
       </c>
       <c r="B18" t="n">
-        <v>1.214233069637331</v>
+        <v>1.214054630626317</v>
       </c>
       <c r="C18" t="n">
         <v>7.163226421827404</v>
@@ -723,7 +723,7 @@
         </is>
       </c>
       <c r="B19" t="n">
-        <v>1.999999999999918</v>
+        <v>1.99999999999919</v>
       </c>
       <c r="C19" t="n">
         <v>2.120000000000013</v>
@@ -739,7 +739,7 @@
         </is>
       </c>
       <c r="B20" t="n">
-        <v>0.2189051292047605</v>
+        <v>0.218895274988578</v>
       </c>
       <c r="C20" t="n">
         <v>0.2446962585405372</v>
@@ -755,7 +755,7 @@
         </is>
       </c>
       <c r="B21" t="n">
-        <v>1.816094870795158</v>
+        <v>1.816104725010612</v>
       </c>
       <c r="C21" t="n">
         <v>1.892303741459475</v>
@@ -771,7 +771,7 @@
         </is>
       </c>
       <c r="B22" t="n">
-        <v>1.819285348705744</v>
+        <v>1.819294851080049</v>
       </c>
       <c r="C22" t="n">
         <v>1.89535013941786</v>
@@ -787,7 +787,7 @@
         </is>
       </c>
       <c r="B23" t="n">
-        <v>0.2189636826515198</v>
+        <v>0.2189538329839706</v>
       </c>
       <c r="C23" t="n">
         <v>0.2447559684514999</v>
@@ -819,7 +819,7 @@
         </is>
       </c>
       <c r="B25" t="n">
-        <v>1.038249015808105</v>
+        <v>1.038248658180237</v>
       </c>
       <c r="C25" t="n">
         <v>1.080106139183044</v>
@@ -835,7 +835,7 @@
         </is>
       </c>
       <c r="B26" t="n">
-        <v>0.1229048114135727</v>
+        <v>0.1228985987824348</v>
       </c>
       <c r="C26" t="n">
         <v>0.1203275423241102</v>
@@ -883,7 +883,7 @@
         </is>
       </c>
       <c r="B29" t="n">
-        <v>104.5951640625</v>
+        <v>104.5975625</v>
       </c>
       <c r="C29" t="n">
         <v>79.60096875000001</v>
@@ -915,7 +915,7 @@
         </is>
       </c>
       <c r="B31" t="n">
-        <v>104.5951676965513</v>
+        <v>104.5975605534461</v>
       </c>
       <c r="C31" t="n">
         <v>79.6009678006568</v>

</xml_diff>

<commit_message>
major update: vectorization of heat and mass transfer components - part 1
</commit_message>
<xml_diff>
--- a/PyScripts/output/validation.xlsx
+++ b/PyScripts/output/validation.xlsx
@@ -451,13 +451,13 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>51005.00823254297</v>
+        <v>51005.00823254327</v>
       </c>
       <c r="C2" t="n">
-        <v>32470.46482413697</v>
+        <v>32470.46581558938</v>
       </c>
       <c r="D2" t="n">
-        <v>30562.23919850059</v>
+        <v>30562.23921417492</v>
       </c>
     </row>
     <row r="3">
@@ -467,13 +467,13 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>32401.14538257632</v>
+        <v>32401.14538257644</v>
       </c>
       <c r="C3" t="n">
-        <v>22890.15223737805</v>
+        <v>22890.15288778509</v>
       </c>
       <c r="D3" t="n">
-        <v>24229.09556265955</v>
+        <v>24229.09556773193</v>
       </c>
     </row>
     <row r="4">
@@ -486,7 +486,7 @@
         <v>30319.8542017977</v>
       </c>
       <c r="C4" t="n">
-        <v>28159.8542017977</v>
+        <v>28159.85420179771</v>
       </c>
       <c r="D4" t="n">
         <v>28159.8542017977</v>
@@ -499,13 +499,13 @@
         </is>
       </c>
       <c r="B5" t="n">
-        <v>2081.291180778615</v>
+        <v>2081.291180778742</v>
       </c>
       <c r="C5" t="n">
-        <v>-5269.701964419652</v>
+        <v>-5269.701314012611</v>
       </c>
       <c r="D5" t="n">
-        <v>-3930.758639138152</v>
+        <v>-3930.758634065773</v>
       </c>
     </row>
     <row r="6">
@@ -515,13 +515,13 @@
         </is>
       </c>
       <c r="B6" t="n">
-        <v>3532.226790597309</v>
+        <v>3532.226790597325</v>
       </c>
       <c r="C6" t="n">
-        <v>603.2279645160052</v>
+        <v>603.228126407048</v>
       </c>
       <c r="D6" t="n">
-        <v>854.6824965449755</v>
+        <v>854.6824980789443</v>
       </c>
     </row>
     <row r="7">
@@ -547,13 +547,13 @@
         </is>
       </c>
       <c r="B8" t="n">
-        <v>1964.726790597309</v>
+        <v>1964.726790597325</v>
       </c>
       <c r="C8" t="n">
-        <v>-964.2720354839948</v>
+        <v>-964.271873592952</v>
       </c>
       <c r="D8" t="n">
-        <v>-712.8175034550245</v>
+        <v>-712.8175019210557</v>
       </c>
     </row>
     <row r="9">
@@ -579,13 +579,13 @@
         </is>
       </c>
       <c r="B10" t="n">
-        <v>26.99999999998431</v>
+        <v>26.9999999999842</v>
       </c>
       <c r="C10" t="n">
-        <v>23.72113514408119</v>
+        <v>23.72113548365826</v>
       </c>
       <c r="D10" t="n">
-        <v>26.79948907117119</v>
+        <v>26.79948907564955</v>
       </c>
     </row>
     <row r="11">
@@ -595,13 +595,13 @@
         </is>
       </c>
       <c r="B11" t="n">
-        <v>26.62374482422558</v>
+        <v>26.62374482422547</v>
       </c>
       <c r="C11" t="n">
-        <v>23.99999999999983</v>
+        <v>23.99999999999966</v>
       </c>
       <c r="D11" t="n">
-        <v>27.0000000000004</v>
+        <v>27.00000000000074</v>
       </c>
     </row>
     <row r="12">
@@ -611,13 +611,13 @@
         </is>
       </c>
       <c r="B12" t="n">
-        <v>27.03821225603286</v>
+        <v>27.03821225603281</v>
       </c>
       <c r="C12" t="n">
-        <v>23.25952019118625</v>
+        <v>23.25952027162458</v>
       </c>
       <c r="D12" t="n">
-        <v>26.34810447416294</v>
+        <v>26.34810447478441</v>
       </c>
     </row>
     <row r="13">
@@ -630,10 +630,10 @@
         <v>64.73487797803335</v>
       </c>
       <c r="C13" t="n">
-        <v>22.31024172486366</v>
+        <v>22.31024220932733</v>
       </c>
       <c r="D13" t="n">
-        <v>25.5907792209062</v>
+        <v>25.59077922640171</v>
       </c>
     </row>
     <row r="14">
@@ -643,13 +643,13 @@
         </is>
       </c>
       <c r="B14" t="n">
-        <v>11.63509226463992</v>
+        <v>11.63509226463964</v>
       </c>
       <c r="C14" t="n">
-        <v>16.04738618027744</v>
+        <v>16.04738583843084</v>
       </c>
       <c r="D14" t="n">
-        <v>16.51352254903583</v>
+        <v>16.51352254582582</v>
       </c>
     </row>
     <row r="15">
@@ -659,13 +659,13 @@
         </is>
       </c>
       <c r="B15" t="n">
-        <v>8.422298003455047</v>
+        <v>8.42229800345512</v>
       </c>
       <c r="C15" t="n">
-        <v>6.578993866641933</v>
+        <v>6.578993731832838</v>
       </c>
       <c r="D15" t="n">
-        <v>6.397913401514893</v>
+        <v>6.397913399830364</v>
       </c>
     </row>
     <row r="16">
@@ -675,13 +675,13 @@
         </is>
       </c>
       <c r="B16" t="n">
-        <v>15.45561770905346</v>
+        <v>15.45561770905357</v>
       </c>
       <c r="C16" t="n">
-        <v>12.46304758374061</v>
+        <v>12.46304758373543</v>
       </c>
       <c r="D16" t="n">
-        <v>12.34675695646267</v>
+        <v>12.34675695646129</v>
       </c>
     </row>
     <row r="17">
@@ -691,13 +691,13 @@
         </is>
       </c>
       <c r="B17" t="n">
-        <v>15.05671624322933</v>
+        <v>15.05671624322941</v>
       </c>
       <c r="C17" t="n">
-        <v>12.99920415303144</v>
+        <v>12.99920408985287</v>
       </c>
       <c r="D17" t="n">
-        <v>12.80326246143624</v>
+        <v>12.80326246096673</v>
       </c>
     </row>
     <row r="18">
@@ -710,10 +710,10 @@
         <v>1.214054630626317</v>
       </c>
       <c r="C18" t="n">
-        <v>7.163226421827404</v>
+        <v>7.163226210294543</v>
       </c>
       <c r="D18" t="n">
-        <v>6.869636926063983</v>
+        <v>6.86963692382496</v>
       </c>
     </row>
     <row r="19">
@@ -723,13 +723,13 @@
         </is>
       </c>
       <c r="B19" t="n">
-        <v>1.99999999999919</v>
+        <v>1.999999999999191</v>
       </c>
       <c r="C19" t="n">
-        <v>2.120000000000013</v>
+        <v>2.120000000000014</v>
       </c>
       <c r="D19" t="n">
-        <v>1.760000000000054</v>
+        <v>1.760000000000049</v>
       </c>
     </row>
     <row r="20">
@@ -739,13 +739,13 @@
         </is>
       </c>
       <c r="B20" t="n">
-        <v>0.218895274988578</v>
+        <v>0.2188952749885781</v>
       </c>
       <c r="C20" t="n">
-        <v>0.2446962585405372</v>
+        <v>0.2446962585474506</v>
       </c>
       <c r="D20" t="n">
-        <v>0.2061140735987233</v>
+        <v>0.2061140735987855</v>
       </c>
     </row>
     <row r="21">
@@ -755,13 +755,13 @@
         </is>
       </c>
       <c r="B21" t="n">
-        <v>1.816104725010612</v>
+        <v>1.816104725010613</v>
       </c>
       <c r="C21" t="n">
-        <v>1.892303741459475</v>
+        <v>1.892303741452564</v>
       </c>
       <c r="D21" t="n">
-        <v>1.570885926401331</v>
+        <v>1.570885926401263</v>
       </c>
     </row>
     <row r="22">
@@ -774,7 +774,7 @@
         <v>1.819294851080049</v>
       </c>
       <c r="C22" t="n">
-        <v>1.89535013941786</v>
+        <v>1.89535013941073</v>
       </c>
       <c r="D22" t="n">
         <v>1.57388701945878</v>
@@ -838,10 +838,10 @@
         <v>0.1228985987824348</v>
       </c>
       <c r="C26" t="n">
-        <v>0.1203275423241102</v>
+        <v>0.1203275423282032</v>
       </c>
       <c r="D26" t="n">
-        <v>0.1203868915115663</v>
+        <v>0.1203868915116111</v>
       </c>
     </row>
     <row r="27">
@@ -918,10 +918,10 @@
         <v>104.5975605534461</v>
       </c>
       <c r="C31" t="n">
-        <v>79.6009678006568</v>
+        <v>79.60096779650935</v>
       </c>
       <c r="D31" t="n">
-        <v>78.59142710051891</v>
+        <v>78.5914271004912</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
vectorization part 2: TubeConduction and WallConduction + adapeted and tested aircraft model
</commit_message>
<xml_diff>
--- a/PyScripts/output/validation.xlsx
+++ b/PyScripts/output/validation.xlsx
@@ -451,13 +451,13 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>51005.00823254327</v>
+        <v>51005.00823254132</v>
       </c>
       <c r="C2" t="n">
-        <v>32470.46581558938</v>
+        <v>32470.46580871383</v>
       </c>
       <c r="D2" t="n">
-        <v>30562.23921417492</v>
+        <v>30562.23921417497</v>
       </c>
     </row>
     <row r="3">
@@ -467,13 +467,13 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>32401.14538257644</v>
+        <v>32401.14538257608</v>
       </c>
       <c r="C3" t="n">
-        <v>22890.15288778509</v>
+        <v>22890.15288778023</v>
       </c>
       <c r="D3" t="n">
-        <v>24229.09556773193</v>
+        <v>24229.09556773915</v>
       </c>
     </row>
     <row r="4">
@@ -499,13 +499,13 @@
         </is>
       </c>
       <c r="B5" t="n">
-        <v>2081.291180778742</v>
+        <v>2081.291180778378</v>
       </c>
       <c r="C5" t="n">
-        <v>-5269.701314012611</v>
+        <v>-5269.701314017479</v>
       </c>
       <c r="D5" t="n">
-        <v>-3930.758634065773</v>
+        <v>-3930.758634058555</v>
       </c>
     </row>
     <row r="6">
@@ -515,13 +515,13 @@
         </is>
       </c>
       <c r="B6" t="n">
-        <v>3532.226790597325</v>
+        <v>3532.226790597284</v>
       </c>
       <c r="C6" t="n">
-        <v>603.228126407048</v>
+        <v>603.2281264111161</v>
       </c>
       <c r="D6" t="n">
-        <v>854.6824980789443</v>
+        <v>854.6824980921797</v>
       </c>
     </row>
     <row r="7">
@@ -547,13 +547,13 @@
         </is>
       </c>
       <c r="B8" t="n">
-        <v>1964.726790597325</v>
+        <v>1964.726790597284</v>
       </c>
       <c r="C8" t="n">
-        <v>-964.271873592952</v>
+        <v>-964.2718735888839</v>
       </c>
       <c r="D8" t="n">
-        <v>-712.8175019210557</v>
+        <v>-712.8175019078203</v>
       </c>
     </row>
     <row r="9">
@@ -582,10 +582,10 @@
         <v>26.9999999999842</v>
       </c>
       <c r="C10" t="n">
-        <v>23.72113548365826</v>
+        <v>23.72113548365832</v>
       </c>
       <c r="D10" t="n">
-        <v>26.79948907564955</v>
+        <v>26.79948907564994</v>
       </c>
     </row>
     <row r="11">
@@ -617,7 +617,7 @@
         <v>23.25952027162458</v>
       </c>
       <c r="D12" t="n">
-        <v>26.34810447478441</v>
+        <v>26.34810447478401</v>
       </c>
     </row>
     <row r="13">
@@ -633,7 +633,7 @@
         <v>22.31024220932733</v>
       </c>
       <c r="D13" t="n">
-        <v>25.59077922640171</v>
+        <v>25.59077922640409</v>
       </c>
     </row>
     <row r="14">
@@ -643,13 +643,13 @@
         </is>
       </c>
       <c r="B14" t="n">
-        <v>11.63509226463964</v>
+        <v>11.63509226463987</v>
       </c>
       <c r="C14" t="n">
         <v>16.04738583843084</v>
       </c>
       <c r="D14" t="n">
-        <v>16.51352254582582</v>
+        <v>16.51352254582577</v>
       </c>
     </row>
     <row r="15">
@@ -659,13 +659,13 @@
         </is>
       </c>
       <c r="B15" t="n">
-        <v>8.42229800345512</v>
+        <v>8.42229800345515</v>
       </c>
       <c r="C15" t="n">
-        <v>6.578993731832838</v>
+        <v>6.578993731832816</v>
       </c>
       <c r="D15" t="n">
-        <v>6.397913399830364</v>
+        <v>6.397913399825484</v>
       </c>
     </row>
     <row r="16">
@@ -681,7 +681,7 @@
         <v>12.46304758373543</v>
       </c>
       <c r="D16" t="n">
-        <v>12.34675695646129</v>
+        <v>12.34675695646256</v>
       </c>
     </row>
     <row r="17">
@@ -697,7 +697,7 @@
         <v>12.99920408985287</v>
       </c>
       <c r="D17" t="n">
-        <v>12.80326246096673</v>
+        <v>12.80326246096684</v>
       </c>
     </row>
     <row r="18">
@@ -707,13 +707,13 @@
         </is>
       </c>
       <c r="B18" t="n">
-        <v>1.214054630626317</v>
+        <v>1.214054630626322</v>
       </c>
       <c r="C18" t="n">
-        <v>7.163226210294543</v>
+        <v>7.163226210294542</v>
       </c>
       <c r="D18" t="n">
-        <v>6.86963692382496</v>
+        <v>6.869636923817704</v>
       </c>
     </row>
     <row r="19">
@@ -723,13 +723,13 @@
         </is>
       </c>
       <c r="B19" t="n">
-        <v>1.999999999999191</v>
+        <v>1.99999999999919</v>
       </c>
       <c r="C19" t="n">
-        <v>2.120000000000014</v>
+        <v>2.120000000000028</v>
       </c>
       <c r="D19" t="n">
-        <v>1.760000000000049</v>
+        <v>1.76000000000005</v>
       </c>
     </row>
     <row r="20">
@@ -739,13 +739,13 @@
         </is>
       </c>
       <c r="B20" t="n">
-        <v>0.2188952749885781</v>
+        <v>0.218895274988578</v>
       </c>
       <c r="C20" t="n">
-        <v>0.2446962585474506</v>
+        <v>0.2446962585474512</v>
       </c>
       <c r="D20" t="n">
-        <v>0.2061140735987855</v>
+        <v>0.2061140735987845</v>
       </c>
     </row>
     <row r="21">
@@ -755,13 +755,13 @@
         </is>
       </c>
       <c r="B21" t="n">
-        <v>1.816104725010613</v>
+        <v>1.816104725010612</v>
       </c>
       <c r="C21" t="n">
-        <v>1.892303741452564</v>
+        <v>1.892303741452576</v>
       </c>
       <c r="D21" t="n">
-        <v>1.570885926401263</v>
+        <v>1.570885926401265</v>
       </c>
     </row>
     <row r="22">
@@ -774,10 +774,10 @@
         <v>1.819294851080049</v>
       </c>
       <c r="C22" t="n">
-        <v>1.89535013941073</v>
+        <v>1.895350139410584</v>
       </c>
       <c r="D22" t="n">
-        <v>1.57388701945878</v>
+        <v>1.573887019458925</v>
       </c>
     </row>
     <row r="23">
@@ -838,10 +838,10 @@
         <v>0.1228985987824348</v>
       </c>
       <c r="C26" t="n">
-        <v>0.1203275423282032</v>
+        <v>0.1203275423282027</v>
       </c>
       <c r="D26" t="n">
-        <v>0.1203868915116111</v>
+        <v>0.1203868915116103</v>
       </c>
     </row>
     <row r="27">
@@ -918,7 +918,7 @@
         <v>104.5975605534461</v>
       </c>
       <c r="C31" t="n">
-        <v>79.60096779650935</v>
+        <v>79.60096779650938</v>
       </c>
       <c r="D31" t="n">
         <v>78.5914271004912</v>

</xml_diff>

<commit_message>
manual revert to un-vectorized version of the library
</commit_message>
<xml_diff>
--- a/PyScripts/output/validation.xlsx
+++ b/PyScripts/output/validation.xlsx
@@ -451,13 +451,13 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>51005.00823254132</v>
+        <v>51005.00823254297</v>
       </c>
       <c r="C2" t="n">
-        <v>32470.46580871383</v>
+        <v>32470.46482413697</v>
       </c>
       <c r="D2" t="n">
-        <v>30562.23921417497</v>
+        <v>30562.23919850059</v>
       </c>
     </row>
     <row r="3">
@@ -467,13 +467,13 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>32401.14538257608</v>
+        <v>32401.14538257632</v>
       </c>
       <c r="C3" t="n">
-        <v>22890.15288778023</v>
+        <v>22890.15223737805</v>
       </c>
       <c r="D3" t="n">
-        <v>24229.09556773915</v>
+        <v>24229.09556265955</v>
       </c>
     </row>
     <row r="4">
@@ -486,7 +486,7 @@
         <v>30319.8542017977</v>
       </c>
       <c r="C4" t="n">
-        <v>28159.85420179771</v>
+        <v>28159.8542017977</v>
       </c>
       <c r="D4" t="n">
         <v>28159.8542017977</v>
@@ -499,13 +499,13 @@
         </is>
       </c>
       <c r="B5" t="n">
-        <v>2081.291180778378</v>
+        <v>2081.291180778615</v>
       </c>
       <c r="C5" t="n">
-        <v>-5269.701314017479</v>
+        <v>-5269.701964419652</v>
       </c>
       <c r="D5" t="n">
-        <v>-3930.758634058555</v>
+        <v>-3930.758639138152</v>
       </c>
     </row>
     <row r="6">
@@ -515,13 +515,13 @@
         </is>
       </c>
       <c r="B6" t="n">
-        <v>3532.226790597284</v>
+        <v>3532.226790597309</v>
       </c>
       <c r="C6" t="n">
-        <v>603.2281264111161</v>
+        <v>603.2279645160052</v>
       </c>
       <c r="D6" t="n">
-        <v>854.6824980921797</v>
+        <v>854.6824965449755</v>
       </c>
     </row>
     <row r="7">
@@ -547,13 +547,13 @@
         </is>
       </c>
       <c r="B8" t="n">
-        <v>1964.726790597284</v>
+        <v>1964.726790597309</v>
       </c>
       <c r="C8" t="n">
-        <v>-964.2718735888839</v>
+        <v>-964.2720354839948</v>
       </c>
       <c r="D8" t="n">
-        <v>-712.8175019078203</v>
+        <v>-712.8175034550245</v>
       </c>
     </row>
     <row r="9">
@@ -579,13 +579,13 @@
         </is>
       </c>
       <c r="B10" t="n">
-        <v>26.9999999999842</v>
+        <v>26.99999999998431</v>
       </c>
       <c r="C10" t="n">
-        <v>23.72113548365832</v>
+        <v>23.72113514408119</v>
       </c>
       <c r="D10" t="n">
-        <v>26.79948907564994</v>
+        <v>26.79948907117119</v>
       </c>
     </row>
     <row r="11">
@@ -595,13 +595,13 @@
         </is>
       </c>
       <c r="B11" t="n">
-        <v>26.62374482422547</v>
+        <v>26.62374482422558</v>
       </c>
       <c r="C11" t="n">
-        <v>23.99999999999966</v>
+        <v>23.99999999999983</v>
       </c>
       <c r="D11" t="n">
-        <v>27.00000000000074</v>
+        <v>27.0000000000004</v>
       </c>
     </row>
     <row r="12">
@@ -611,13 +611,13 @@
         </is>
       </c>
       <c r="B12" t="n">
-        <v>27.03821225603281</v>
+        <v>27.03821225603286</v>
       </c>
       <c r="C12" t="n">
-        <v>23.25952027162458</v>
+        <v>23.25952019118625</v>
       </c>
       <c r="D12" t="n">
-        <v>26.34810447478401</v>
+        <v>26.34810447416294</v>
       </c>
     </row>
     <row r="13">
@@ -630,10 +630,10 @@
         <v>64.73487797803335</v>
       </c>
       <c r="C13" t="n">
-        <v>22.31024220932733</v>
+        <v>22.31024172486366</v>
       </c>
       <c r="D13" t="n">
-        <v>25.59077922640409</v>
+        <v>25.5907792209062</v>
       </c>
     </row>
     <row r="14">
@@ -643,13 +643,13 @@
         </is>
       </c>
       <c r="B14" t="n">
-        <v>11.63509226463987</v>
+        <v>11.63509226463992</v>
       </c>
       <c r="C14" t="n">
-        <v>16.04738583843084</v>
+        <v>16.04738618027744</v>
       </c>
       <c r="D14" t="n">
-        <v>16.51352254582577</v>
+        <v>16.51352254903583</v>
       </c>
     </row>
     <row r="15">
@@ -659,13 +659,13 @@
         </is>
       </c>
       <c r="B15" t="n">
-        <v>8.42229800345515</v>
+        <v>8.422298003455047</v>
       </c>
       <c r="C15" t="n">
-        <v>6.578993731832816</v>
+        <v>6.578993866641933</v>
       </c>
       <c r="D15" t="n">
-        <v>6.397913399825484</v>
+        <v>6.397913401514893</v>
       </c>
     </row>
     <row r="16">
@@ -675,13 +675,13 @@
         </is>
       </c>
       <c r="B16" t="n">
-        <v>15.45561770905357</v>
+        <v>15.45561770905346</v>
       </c>
       <c r="C16" t="n">
-        <v>12.46304758373543</v>
+        <v>12.46304758374061</v>
       </c>
       <c r="D16" t="n">
-        <v>12.34675695646256</v>
+        <v>12.34675695646267</v>
       </c>
     </row>
     <row r="17">
@@ -691,13 +691,13 @@
         </is>
       </c>
       <c r="B17" t="n">
-        <v>15.05671624322941</v>
+        <v>15.05671624322933</v>
       </c>
       <c r="C17" t="n">
-        <v>12.99920408985287</v>
+        <v>12.99920415303144</v>
       </c>
       <c r="D17" t="n">
-        <v>12.80326246096684</v>
+        <v>12.80326246143624</v>
       </c>
     </row>
     <row r="18">
@@ -707,13 +707,13 @@
         </is>
       </c>
       <c r="B18" t="n">
-        <v>1.214054630626322</v>
+        <v>1.214054630626317</v>
       </c>
       <c r="C18" t="n">
-        <v>7.163226210294542</v>
+        <v>7.163226421827404</v>
       </c>
       <c r="D18" t="n">
-        <v>6.869636923817704</v>
+        <v>6.869636926063983</v>
       </c>
     </row>
     <row r="19">
@@ -726,10 +726,10 @@
         <v>1.99999999999919</v>
       </c>
       <c r="C19" t="n">
-        <v>2.120000000000028</v>
+        <v>2.120000000000013</v>
       </c>
       <c r="D19" t="n">
-        <v>1.76000000000005</v>
+        <v>1.760000000000054</v>
       </c>
     </row>
     <row r="20">
@@ -742,10 +742,10 @@
         <v>0.218895274988578</v>
       </c>
       <c r="C20" t="n">
-        <v>0.2446962585474512</v>
+        <v>0.2446962585405372</v>
       </c>
       <c r="D20" t="n">
-        <v>0.2061140735987845</v>
+        <v>0.2061140735987233</v>
       </c>
     </row>
     <row r="21">
@@ -758,10 +758,10 @@
         <v>1.816104725010612</v>
       </c>
       <c r="C21" t="n">
-        <v>1.892303741452576</v>
+        <v>1.892303741459475</v>
       </c>
       <c r="D21" t="n">
-        <v>1.570885926401265</v>
+        <v>1.570885926401331</v>
       </c>
     </row>
     <row r="22">
@@ -774,10 +774,10 @@
         <v>1.819294851080049</v>
       </c>
       <c r="C22" t="n">
-        <v>1.895350139410584</v>
+        <v>1.89535013941786</v>
       </c>
       <c r="D22" t="n">
-        <v>1.573887019458925</v>
+        <v>1.57388701945878</v>
       </c>
     </row>
     <row r="23">
@@ -838,10 +838,10 @@
         <v>0.1228985987824348</v>
       </c>
       <c r="C26" t="n">
-        <v>0.1203275423282027</v>
+        <v>0.1203275423241102</v>
       </c>
       <c r="D26" t="n">
-        <v>0.1203868915116103</v>
+        <v>0.1203868915115663</v>
       </c>
     </row>
     <row r="27">
@@ -918,10 +918,10 @@
         <v>104.5975605534461</v>
       </c>
       <c r="C31" t="n">
-        <v>79.60096779650938</v>
+        <v>79.6009678006568</v>
       </c>
       <c r="D31" t="n">
-        <v>78.5914271004912</v>
+        <v>78.59142710051891</v>
       </c>
     </row>
   </sheetData>

</xml_diff>